<commit_message>
Removed Items from Excel_Template.xlsx
</commit_message>
<xml_diff>
--- a/Templates/Excel_Template.xlsx
+++ b/Templates/Excel_Template.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\PycharmProjects\PptPythonTutorial\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\PycharmProjects\PowerPointDesdeExcel\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20440EED-2303-4D0E-A3B3-5C6B9D1C5951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22FA7A8-B9AC-416E-BCF7-989AA2D5875A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1860" windowWidth="29040" windowHeight="18240" xr2:uid="{D40DBC42-031A-4053-95CD-2185F8A1C99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" r:id="rId1"/>
     <sheet name="Listas" sheetId="2" r:id="rId2"/>
-    <sheet name="Resultados_PyCoffeeMax_R340" sheetId="3" r:id="rId3"/>
-    <sheet name="Resultados_PyCoffeeMax_R570" sheetId="4" r:id="rId4"/>
-    <sheet name="Resultados_Finales" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="151">
   <si>
     <t>DISEÑO_DIAPOSITIVA</t>
   </si>
@@ -493,107 +490,14 @@
   </si>
   <si>
     <t>LÍNEAS-OSCURO</t>
-  </si>
-  <si>
-    <t>Periodo</t>
-  </si>
-  <si>
-    <t>Q1 - 2023</t>
-  </si>
-  <si>
-    <t>Q2 - 2023</t>
-  </si>
-  <si>
-    <t>Q3 - 2023</t>
-  </si>
-  <si>
-    <t>Q4 - 2023</t>
-  </si>
-  <si>
-    <t>Q1 - 2024</t>
-  </si>
-  <si>
-    <t>Q2 - 2024</t>
-  </si>
-  <si>
-    <t>Q3 - 2024</t>
-  </si>
-  <si>
-    <t>Q4 - 2024</t>
-  </si>
-  <si>
-    <t>Resultados PyCoffeeMax R340</t>
-  </si>
-  <si>
-    <t>Resultados_PyCoffeeMax_R340</t>
-  </si>
-  <si>
-    <t>PyCoffeeMax R340</t>
-  </si>
-  <si>
-    <t>#9B2D1F</t>
-  </si>
-  <si>
-    <t>Ganancias Brutas (€)</t>
-  </si>
-  <si>
-    <t>Precio Unitario  (€)</t>
-  </si>
-  <si>
-    <t>Ventas (uds.)</t>
-  </si>
-  <si>
-    <t>PyCoffeeMax R570</t>
-  </si>
-  <si>
-    <t>Resultados_PyCoffeeMax_R570</t>
-  </si>
-  <si>
-    <t>#956251</t>
-  </si>
-  <si>
-    <t>Resultados PyCoffeeMax R570</t>
-  </si>
-  <si>
-    <t>Comparación Ventas</t>
-  </si>
-  <si>
-    <t>Total Ganancias Brutas (€)</t>
-  </si>
-  <si>
-    <t>Ventas PyCoffeeMax R340</t>
-  </si>
-  <si>
-    <t>Ventas PyCoffeeMax R570</t>
-  </si>
-  <si>
-    <t>Resultados Finales</t>
-  </si>
-  <si>
-    <t>Resultados_Finales</t>
-  </si>
-  <si>
-    <t>Ganancias Brutas PyCoffee R340 (€)</t>
-  </si>
-  <si>
-    <t>Ganancias Brutas PyCoffee R570 (€)</t>
-  </si>
-  <si>
-    <t>Ganancias Brutas PyCoffee R340 (€), Ganancias Brutas PyCoffee R570 (€), Total Ganancias Brutas (€)</t>
-  </si>
-  <si>
-    <t>#9B2D1F, #956251, #D34817</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;cm&quot;"/>
-    <numFmt numFmtId="165" formatCode="0\ &quot;uds.&quot;"/>
-    <numFmt numFmtId="166" formatCode="[$-C0A]d\ &quot;de&quot;\ mmmm\ &quot;de&quot;\ yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -684,12 +588,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -736,18 +639,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1253,10 +1149,10 @@
   <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z27" sqref="Z27"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1355,359 +1251,132 @@
       <c r="V1" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="W1" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="X1" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Y1" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="Z1" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AA1" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AB1" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AC1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AD1" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AE1" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AF1" s="16" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="4"/>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="D5" s="4" t="s">
-        <v>160</v>
-      </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="D7" s="4"/>
-      <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="6">
-        <v>24</v>
-      </c>
-      <c r="W7" t="s">
-        <v>161</v>
-      </c>
-      <c r="X7" t="s">
-        <v>162</v>
-      </c>
-      <c r="Y7">
-        <v>1</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>136</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>164</v>
-      </c>
-      <c r="AC7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>163</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="8" spans="1:32" ht="15" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D8" s="4"/>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="D11" s="4" t="s">
-        <v>170</v>
-      </c>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="D13" s="4"/>
-      <c r="E13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="6">
-        <v>24</v>
-      </c>
-      <c r="W13" t="s">
-        <v>168</v>
-      </c>
-      <c r="X13" t="s">
-        <v>167</v>
-      </c>
-      <c r="Y13">
-        <v>1</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>136</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>164</v>
-      </c>
-      <c r="AC13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>169</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="14" spans="1:32" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D14" s="4"/>
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="C16" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:32" ht="15" x14ac:dyDescent="0.3">
-      <c r="D17" s="4" t="s">
-        <v>171</v>
-      </c>
+    <row r="17" spans="4:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="D17" s="4"/>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
-        <v>11</v>
-      </c>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D19" s="4"/>
-      <c r="E19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="6">
-        <v>24</v>
-      </c>
-      <c r="W19" t="s">
-        <v>161</v>
-      </c>
-      <c r="X19" t="s">
-        <v>173</v>
-      </c>
-      <c r="Y19">
-        <v>1</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>166</v>
-      </c>
-      <c r="AC19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D21" s="4"/>
-      <c r="E21" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="6">
-        <v>24</v>
-      </c>
-      <c r="W21" t="s">
-        <v>168</v>
-      </c>
-      <c r="X21" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y21">
-        <v>1</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>166</v>
-      </c>
-      <c r="AC21" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B23" s="2">
-        <v>0</v>
-      </c>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="C24" s="2" t="s">
-        <v>20</v>
-      </c>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="D25" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B26" s="2">
-        <v>1</v>
-      </c>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D27" s="4"/>
-      <c r="E27" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" s="6">
-        <v>24</v>
-      </c>
-      <c r="W27" t="s">
-        <v>176</v>
-      </c>
-      <c r="X27" t="s">
-        <v>175</v>
-      </c>
-      <c r="Y27">
-        <v>1</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>179</v>
-      </c>
-      <c r="AC27" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>180</v>
-      </c>
-      <c r="AE27" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.3">
@@ -1847,9 +1516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE280D3-A32D-42F7-A7DB-8602297F25F3}">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2401,642 +2068,4 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3AF0AB-AB7E-47D1-BDBE-1A35DBD51163}">
-  <dimension ref="A1:G16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="19">
-        <v>234</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="17">
-        <v>86</v>
-      </c>
-      <c r="D2" s="17">
-        <f>A2*C2</f>
-        <v>20124</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="19">
-        <v>302</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="17">
-        <v>86</v>
-      </c>
-      <c r="D3" s="17">
-        <f t="shared" ref="D3:D9" si="0">A3*C3</f>
-        <v>25972</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="19">
-        <v>195</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" s="17">
-        <v>86</v>
-      </c>
-      <c r="D4" s="17">
-        <f t="shared" si="0"/>
-        <v>16770</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="19">
-        <v>437</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" s="17">
-        <v>86</v>
-      </c>
-      <c r="D5" s="17">
-        <f t="shared" si="0"/>
-        <v>37582</v>
-      </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="19">
-        <v>322</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" s="17">
-        <v>78</v>
-      </c>
-      <c r="D6" s="17">
-        <f t="shared" si="0"/>
-        <v>25116</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="19">
-        <v>376</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" s="17">
-        <v>78</v>
-      </c>
-      <c r="D7" s="17">
-        <f t="shared" si="0"/>
-        <v>29328</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
-        <v>304</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8" s="17">
-        <v>78</v>
-      </c>
-      <c r="D8" s="17">
-        <f t="shared" si="0"/>
-        <v>23712</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
-        <v>576</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" s="17">
-        <v>78</v>
-      </c>
-      <c r="D9" s="17">
-        <f t="shared" si="0"/>
-        <v>44928</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCFBA0AC-F7D4-4295-949E-81EF67386B70}">
-  <dimension ref="A1:G16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="19">
-        <v>256</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="17">
-        <v>123.99</v>
-      </c>
-      <c r="D2" s="17">
-        <f>A2*C2</f>
-        <v>31741.439999999999</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="19">
-        <v>41</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="17">
-        <v>123.99</v>
-      </c>
-      <c r="D3" s="17">
-        <f t="shared" ref="D3:D9" si="0">A3*C3</f>
-        <v>5083.59</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="19">
-        <v>29</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" s="17">
-        <v>123.99</v>
-      </c>
-      <c r="D4" s="17">
-        <f t="shared" si="0"/>
-        <v>3595.71</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="19">
-        <v>12</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" s="17">
-        <v>123.99</v>
-      </c>
-      <c r="D5" s="17">
-        <f t="shared" si="0"/>
-        <v>1487.8799999999999</v>
-      </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="19">
-        <v>138</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" s="17">
-        <v>129.99</v>
-      </c>
-      <c r="D6" s="17">
-        <f t="shared" si="0"/>
-        <v>17938.620000000003</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="19">
-        <v>400</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" s="17">
-        <v>129.99</v>
-      </c>
-      <c r="D7" s="17">
-        <f t="shared" si="0"/>
-        <v>51996</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
-        <v>12</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8" s="17">
-        <v>129.99</v>
-      </c>
-      <c r="D8" s="17">
-        <f t="shared" si="0"/>
-        <v>1559.88</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
-        <v>235</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" s="17">
-        <v>129.99</v>
-      </c>
-      <c r="D9" s="17">
-        <f t="shared" si="0"/>
-        <v>30547.65</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AA7BD9-92F0-4285-A3F2-FFFB3B7B7EBF}">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" s="17">
-        <f>VLOOKUP(A2,Resultados_PyCoffeeMax_R340!B1:D9,3,FALSE)</f>
-        <v>20124</v>
-      </c>
-      <c r="C2" s="17">
-        <f>VLOOKUP(A2,Resultados_PyCoffeeMax_R570!B1:D9,3,FALSE)</f>
-        <v>31741.439999999999</v>
-      </c>
-      <c r="D2" s="22">
-        <f>B2+C2</f>
-        <v>51865.440000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B3" s="17">
-        <f>VLOOKUP(A3,Resultados_PyCoffeeMax_R340!B2:D10,3,FALSE)</f>
-        <v>25972</v>
-      </c>
-      <c r="C3" s="17">
-        <f>VLOOKUP(A3,Resultados_PyCoffeeMax_R570!B2:D10,3,FALSE)</f>
-        <v>5083.59</v>
-      </c>
-      <c r="D3" s="22">
-        <f t="shared" ref="D3:D9" si="0">B3+C3</f>
-        <v>31055.59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" s="17">
-        <f>VLOOKUP(A4,Resultados_PyCoffeeMax_R340!B3:D11,3,FALSE)</f>
-        <v>16770</v>
-      </c>
-      <c r="C4" s="17">
-        <f>VLOOKUP(A4,Resultados_PyCoffeeMax_R570!B3:D11,3,FALSE)</f>
-        <v>3595.71</v>
-      </c>
-      <c r="D4" s="22">
-        <f t="shared" si="0"/>
-        <v>20365.71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" s="17">
-        <f>VLOOKUP(A5,Resultados_PyCoffeeMax_R340!B4:D12,3,FALSE)</f>
-        <v>37582</v>
-      </c>
-      <c r="C5" s="17">
-        <f>VLOOKUP(A5,Resultados_PyCoffeeMax_R570!B4:D12,3,FALSE)</f>
-        <v>1487.8799999999999</v>
-      </c>
-      <c r="D5" s="22">
-        <f t="shared" si="0"/>
-        <v>39069.879999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>156</v>
-      </c>
-      <c r="B6" s="17">
-        <f>VLOOKUP(A6,Resultados_PyCoffeeMax_R340!B5:D13,3,FALSE)</f>
-        <v>25116</v>
-      </c>
-      <c r="C6" s="17">
-        <f>VLOOKUP(A6,Resultados_PyCoffeeMax_R570!B5:D13,3,FALSE)</f>
-        <v>17938.620000000003</v>
-      </c>
-      <c r="D6" s="22">
-        <f t="shared" si="0"/>
-        <v>43054.62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" s="17">
-        <f>VLOOKUP(A7,Resultados_PyCoffeeMax_R340!B6:D14,3,FALSE)</f>
-        <v>29328</v>
-      </c>
-      <c r="C7" s="17">
-        <f>VLOOKUP(A7,Resultados_PyCoffeeMax_R570!B6:D14,3,FALSE)</f>
-        <v>51996</v>
-      </c>
-      <c r="D7" s="22">
-        <f t="shared" si="0"/>
-        <v>81324</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="17">
-        <f>VLOOKUP(A8,Resultados_PyCoffeeMax_R340!B7:D15,3,FALSE)</f>
-        <v>23712</v>
-      </c>
-      <c r="C8" s="17">
-        <f>VLOOKUP(A8,Resultados_PyCoffeeMax_R570!B7:D15,3,FALSE)</f>
-        <v>1559.88</v>
-      </c>
-      <c r="D8" s="22">
-        <f t="shared" si="0"/>
-        <v>25271.88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" s="17">
-        <f>VLOOKUP(A9,Resultados_PyCoffeeMax_R340!B8:D16,3,FALSE)</f>
-        <v>44928</v>
-      </c>
-      <c r="C9" s="17">
-        <f>VLOOKUP(A9,Resultados_PyCoffeeMax_R570!B8:D16,3,FALSE)</f>
-        <v>30547.65</v>
-      </c>
-      <c r="D9" s="22">
-        <f t="shared" si="0"/>
-        <v>75475.649999999994</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add date format to template.
</commit_message>
<xml_diff>
--- a/Templates/Excel_Template.xlsx
+++ b/Templates/Excel_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\PycharmProjects\PowerPointDesdeExcel\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22FA7A8-B9AC-416E-BCF7-989AA2D5875A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE6B6E7-3FB0-41B5-9E62-B338887719E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1860" windowWidth="29040" windowHeight="18240" xr2:uid="{D40DBC42-031A-4053-95CD-2185F8A1C99B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="159">
   <si>
     <t>DISEÑO_DIAPOSITIVA</t>
   </si>
@@ -490,6 +490,30 @@
   </si>
   <si>
     <t>LÍNEAS-OSCURO</t>
+  </si>
+  <si>
+    <t>FORMATO_FECHA</t>
+  </si>
+  <si>
+    <t>dd/mm/yyyy</t>
+  </si>
+  <si>
+    <t>mm/dd/yyyy</t>
+  </si>
+  <si>
+    <t>dd-mmm-yyyy</t>
+  </si>
+  <si>
+    <t>yyyy-mm-dd</t>
+  </si>
+  <si>
+    <t>d de mmm de yyyy</t>
+  </si>
+  <si>
+    <t>dd/mmm/yyyy hh:mm</t>
+  </si>
+  <si>
+    <t>dd-mmm-yyyy hh:mm</t>
   </si>
 </sst>
 </file>
@@ -1514,9 +1538,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE280D3-A32D-42F7-A7DB-8602297F25F3}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1525,9 +1551,10 @@
     <col min="4" max="4" width="34.109375" customWidth="1"/>
     <col min="7" max="7" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1558,8 +1585,11 @@
       <c r="J1" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1590,8 +1620,11 @@
       <c r="J2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1622,8 +1655,11 @@
       <c r="J3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1651,8 +1687,11 @@
       <c r="J4" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1671,8 +1710,11 @@
       <c r="J5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1688,8 +1730,11 @@
       <c r="J6" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1699,8 +1744,11 @@
       <c r="J7" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1710,8 +1758,11 @@
       <c r="J8" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1719,7 +1770,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1727,7 +1778,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1735,7 +1786,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1743,7 +1794,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1751,7 +1802,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1759,12 +1810,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G16" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
Bug fixed: check if 'posicion' is in dictionary. Updated Excel_Template.xlsx to include "FORMATO" within "LISTAS" worksheet.
</commit_message>
<xml_diff>
--- a/Templates/Excel_Template.xlsx
+++ b/Templates/Excel_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\PycharmProjects\PowerPointDesdeExcel\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE6B6E7-3FB0-41B5-9E62-B338887719E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0B8E26-EDED-414F-96A5-83D67B527686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1860" windowWidth="29040" windowHeight="18240" xr2:uid="{D40DBC42-031A-4053-95CD-2185F8A1C99B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D40DBC42-031A-4053-95CD-2185F8A1C99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="165">
   <si>
     <t>DISEÑO_DIAPOSITIVA</t>
   </si>
@@ -514,6 +514,24 @@
   </si>
   <si>
     <t>dd-mmm-yyyy hh:mm</t>
+  </si>
+  <si>
+    <t>FORMATOS</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>decimales</t>
+  </si>
+  <si>
+    <t>sep_decimal</t>
+  </si>
+  <si>
+    <t>simbolo</t>
+  </si>
+  <si>
+    <t>posicion</t>
   </si>
 </sst>
 </file>
@@ -1538,11 +1556,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE280D3-A32D-42F7-A7DB-8602297F25F3}">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1551,10 +1567,10 @@
     <col min="4" max="4" width="34.109375" customWidth="1"/>
     <col min="7" max="7" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1588,8 +1604,11 @@
       <c r="K1" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1623,8 +1642,11 @@
       <c r="K2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1658,8 +1680,11 @@
       <c r="K3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1690,8 +1715,11 @@
       <c r="K4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1713,8 +1741,11 @@
       <c r="K5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1733,8 +1764,11 @@
       <c r="K6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1748,7 +1782,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1762,7 +1796,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1770,7 +1804,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1778,7 +1812,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1786,7 +1820,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1794,7 +1828,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1802,7 +1836,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1810,12 +1844,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G16" t="s">
         <v>67</v>
       </c>

</xml_diff>